<commit_message>
se actualizo la elicitacion de requisitos
</commit_message>
<xml_diff>
--- a/Desarrollo/SDD/Elicitacion de Requisitos.xlsx
+++ b/Desarrollo/SDD/Elicitacion de Requisitos.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neptali Antony Reyes\Desktop\GCS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6060"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="91">
   <si>
     <t>LISTA DE REQUISITOS DEL SISTEMA XYZ</t>
   </si>
@@ -182,9 +177,6 @@
     <t xml:space="preserve">Enviar el horario al correo del docente </t>
   </si>
   <si>
-    <t>Modificar contraseña</t>
-  </si>
-  <si>
     <t>Salir de la aplicación web</t>
   </si>
   <si>
@@ -197,21 +189,12 @@
     <t>RQ22</t>
   </si>
   <si>
-    <t>RQ23</t>
-  </si>
-  <si>
-    <t>RQ24</t>
-  </si>
-  <si>
     <t>Profesor</t>
   </si>
   <si>
     <t>Generar reporte</t>
   </si>
   <si>
-    <t>Editar información personal</t>
-  </si>
-  <si>
     <t>Seleccionar cursos</t>
   </si>
   <si>
@@ -240,9 +223,6 @@
   </si>
   <si>
     <t>El sistema permite que al pulsar el botón “enviar a mail” se envía un correo electrónico, de la base de datos del profesor, con todos sus atributos.</t>
-  </si>
-  <si>
-    <t> Una vez que el docente ha seleccionado su información en el botón  “cambiar contraseña” donde aparece una nueva vista con dos campos para escribir la nueva contraseña y verificar contraseña,  y al pulsar el botón aceptar siempre  y cuando las contraseñas sean iguales cambiará la contraseña de acceso.</t>
   </si>
   <si>
     <r>
@@ -271,15 +251,6 @@
     <t>Verificar si el docente está registrado en la base de datos</t>
   </si>
   <si>
-    <t xml:space="preserve">Ingresar datos del docente </t>
-  </si>
-  <si>
-    <t>Editar datos del docente</t>
-  </si>
-  <si>
-    <t>Registrar datos del docente</t>
-  </si>
-  <si>
     <t>Seleccionar la modalidad del docente ya sea tiempo completo o parcial</t>
   </si>
   <si>
@@ -301,9 +272,6 @@
     <t>Verificar si el docente está registrado</t>
   </si>
   <si>
-    <t>Ingresar datos del docente</t>
-  </si>
-  <si>
     <t>Seleccionar la modalidad del docente</t>
   </si>
   <si>
@@ -316,19 +284,31 @@
     <t>Indicar al docente si las horas marcadas corresponden con su modalidad</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Registro docente</t>
-  </si>
-  <si>
-    <t>Registro disponibilidad</t>
+    <t>Iniciar sesion</t>
+  </si>
+  <si>
+    <t>Editar perfil</t>
+  </si>
+  <si>
+    <t>Registrar disponibilidad</t>
+  </si>
+  <si>
+    <t>Modificar número telefónico</t>
+  </si>
+  <si>
+    <t>Modificar correo</t>
+  </si>
+  <si>
+    <t> Una vez que el docente ha seleccionado la opción  “Editar perfil” donde aparece una nueva vista con un formulario de sus datos, puede modificar su correo si es que asi lo desee.</t>
+  </si>
+  <si>
+    <t> Una vez que el docente ha seleccionado la opción  “Editar perfil” donde aparece una nueva vista con un formulario de sus datos, puede modificar su número de teléfono si es que asi lo desee.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -620,7 +600,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -661,6 +641,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -700,38 +713,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1065,7 +1048,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1100,7 +1083,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1309,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1322,18 +1305,18 @@
     <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="62.140625" customWidth="1"/>
-    <col min="6" max="6" width="50.85546875" customWidth="1"/>
+    <col min="6" max="6" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -1367,16 +1350,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>75</v>
+        <v>56</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1385,16 +1368,16 @@
         <v>12</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>76</v>
+        <v>56</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1403,52 +1386,52 @@
         <v>14</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="41" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1457,16 +1440,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="41" t="s">
-        <v>80</v>
+      <c r="F9" s="29" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1475,16 +1458,16 @@
         <v>18</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>81</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1493,16 +1476,16 @@
         <v>19</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>82</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1511,16 +1494,16 @@
         <v>20</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>83</v>
+        <v>56</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1529,264 +1512,229 @@
         <v>21</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>95</v>
+      <c r="C15" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="33" t="s">
-        <v>62</v>
+      <c r="C17" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="D17" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="33" t="s">
-        <v>62</v>
+      <c r="C18" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="37" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="33" t="s">
-        <v>62</v>
+      <c r="C19" s="21" t="s">
+        <v>57</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="34" t="s">
-        <v>60</v>
+      <c r="C20" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="33" t="s">
-        <v>60</v>
+      <c r="C21" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="33" t="s">
-        <v>60</v>
+      <c r="C22" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
+        <v>56</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="33" t="s">
-        <v>60</v>
+      <c r="C23" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" s="38" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+      <c r="C25" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="34" t="s">
+      <c r="E25" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" s="40" t="s">
-        <v>74</v>
+      <c r="F25" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1821,14 +1769,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1873,10 +1821,10 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="36" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -1885,13 +1833,13 @@
       <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="41">
         <v>2</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="33" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1900,30 +1848,30 @@
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="23"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="24"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -2334,7 +2282,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2344,12 +2292,12 @@
       </c>
     </row>
     <row r="90" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="35" t="s">
+      <c r="B90" s="22" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="128" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B128" s="35" t="s">
+      <c r="B128" s="22" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>